<commit_message>
preenchendo formulario web dados em planilha excell
</commit_message>
<xml_diff>
--- a/Udemy_24/Autom-Python/buscacep.xlsx
+++ b/Udemy_24/Autom-Python/buscacep.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ludwig\Desktop\git-repo\alpha\Udemy_24\Autom-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C531BC2-179A-45A4-852D-80F2F9F753C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1FB461-9EA3-4522-86EE-C2F3DEBA95FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="cep_a_buscar" sheetId="1" r:id="rId1"/>
+    <sheet name="cep_a_consultar" sheetId="1" r:id="rId1"/>
     <sheet name="dados_coletados" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="18">
   <si>
     <t>CEPs a buscar</t>
   </si>
@@ -38,16 +38,43 @@
     <t>CEP</t>
   </si>
   <si>
-    <t xml:space="preserve">Rua Bernardino Fonseca </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tabajaras </t>
+    <t xml:space="preserve">Rua Albertino Silva </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presidente Roosevelt </t>
   </si>
   <si>
     <t xml:space="preserve">Uberlândia/MG </t>
   </si>
   <si>
-    <t>38400-220</t>
+    <t>38401-220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua João Catanduva </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santa Mônica </t>
+  </si>
+  <si>
+    <t>38408-240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua São Paulo - de 157/158 a 1569/1570 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brasil </t>
+  </si>
+  <si>
+    <t>38400-656</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Amador Lourenço </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laranjeiras </t>
+  </si>
+  <si>
+    <t>38410-234</t>
   </si>
 </sst>
 </file>
@@ -430,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,17 +473,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>38401220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38408240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>38400656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>38410234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,6 +543,160 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>